<commit_message>
Alterando anos de comparação 2024-2025
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.reis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.reis\Desktop\Automação\Automação Tom Ticket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58C84F8-DE6C-4E6E-916B-F0AAEDA53DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A3B82-291F-498D-8331-B9C86A565F9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="Comparativo" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparativo Detalhado" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$6:$X$6</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t>Relatório Detalhado</t>
   </si>
@@ -110,9 +111,6 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>2023</t>
-  </si>
-  <si>
     <t>2024</t>
   </si>
   <si>
@@ -156,6 +154,162 @@
   </si>
   <si>
     <t>data de emissão do relatório</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Verba</t>
+  </si>
+  <si>
+    <t>Permissões</t>
+  </si>
+  <si>
+    <t>Acesso á Obra</t>
+  </si>
+  <si>
+    <t>Criar Usuário</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Ativar/Desativar Usuário</t>
+  </si>
+  <si>
+    <t>Treinamento</t>
+  </si>
+  <si>
+    <t>Configurações</t>
+  </si>
+  <si>
+    <t>Relatórios</t>
+  </si>
+  <si>
+    <t>Planejamento</t>
+  </si>
+  <si>
+    <t>Aprovações</t>
+  </si>
+  <si>
+    <t>Abertura Empresa Vinc/Fiscal - Padrão (terça e quinta)</t>
+  </si>
+  <si>
+    <t>Erro Financeiro</t>
+  </si>
+  <si>
+    <t>Criar Obra</t>
+  </si>
+  <si>
+    <t>PRN</t>
+  </si>
+  <si>
+    <t>Dúvida</t>
+  </si>
+  <si>
+    <t>Abertura Empresa Vinc/Fiscal - Esporádico (urgentes)</t>
+  </si>
+  <si>
+    <t>Erro Fiscal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Erro Caixa de Obra</t>
+  </si>
+  <si>
+    <t>Diário de Obra</t>
+  </si>
+  <si>
+    <t>Chamado Técnico de T.I</t>
+  </si>
+  <si>
+    <t>Parametrização Das Obras</t>
+  </si>
+  <si>
+    <t>Solicitar alteração e/ou troca de senha</t>
+  </si>
+  <si>
+    <t>Erro Medição</t>
+  </si>
+  <si>
+    <t>Criar Usuário Remoto (Usuário de Rede)</t>
+  </si>
+  <si>
+    <t>Erro Pedido de Compra</t>
+  </si>
+  <si>
+    <t>UAU Mobile</t>
+  </si>
+  <si>
+    <t>Erro - Modulo  Vendas</t>
+  </si>
+  <si>
+    <t>Manutenção de Computador</t>
+  </si>
+  <si>
+    <t>Erro Requisição</t>
+  </si>
+  <si>
+    <t>Erro Contrato</t>
+  </si>
+  <si>
+    <t>Vinculo Folha</t>
+  </si>
+  <si>
+    <t>Erro-Módulo Obras</t>
+  </si>
+  <si>
+    <t>Reuniões</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>Inconsistência</t>
+  </si>
+  <si>
+    <t>Fechamento de Mês</t>
+  </si>
+  <si>
+    <t>Percentagem Parceria</t>
+  </si>
+  <si>
+    <t>vazio</t>
+  </si>
+  <si>
+    <t>Abertura Empresa Vinc/Fiscal</t>
+  </si>
+  <si>
+    <t>Aplicação de Material</t>
+  </si>
+  <si>
+    <t>Atualização Sistema</t>
+  </si>
+  <si>
+    <t>Acompanhamento Globaltec</t>
+  </si>
+  <si>
+    <t>Derrubar Conexão</t>
+  </si>
+  <si>
+    <t>Problemas com Serviços do Google (Email / Google Drive / Google Meet)</t>
+  </si>
+  <si>
+    <t>Contabilidade</t>
+  </si>
+  <si>
+    <t>Manutenção de Impressora</t>
+  </si>
+  <si>
+    <t>Ficha de Estoque</t>
+  </si>
+  <si>
+    <t>Recuperação de Dados (Backup)</t>
+  </si>
+  <si>
+    <t>InfoUAU</t>
   </si>
 </sst>
 </file>
@@ -191,7 +345,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,11 +364,43 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -223,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -236,6 +422,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +739,7 @@
   <dimension ref="A1:X428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +824,7 @@
     </row>
     <row r="3" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -659,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -7315,7 +7511,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7328,13 +7524,13 @@
         <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -7342,7 +7538,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -7350,7 +7546,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -7358,7 +7554,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -7366,7 +7562,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -7374,7 +7570,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -7382,7 +7578,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -7390,7 +7586,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -7398,7 +7594,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -7406,7 +7602,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -7414,7 +7610,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -7422,7 +7618,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -7443,4 +7639,377 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433B9033-0006-4E4F-8F1A-2D9D4B4CB0E6}">
+  <dimension ref="A1:BD25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD1" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="19">
+        <v>2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>